<commit_message>
Testcases, some fixes to product detail view
minimal changes to use cases
</commit_message>
<xml_diff>
--- a/doc/02 Organisation/Zeiterfassung.xlsx
+++ b/doc/02 Organisation/Zeiterfassung.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="45">
   <si>
     <t>Datum</t>
   </si>
@@ -151,6 +151,9 @@
   </si>
   <si>
     <t>Produktansichten implementiert</t>
+  </si>
+  <si>
+    <t>Testfälle erstellt, Fehlerbehebung</t>
   </si>
 </sst>
 </file>
@@ -568,10 +571,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B3:E45"/>
+  <dimension ref="B3:E49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E45" sqref="E45"/>
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1181,6 +1184,62 @@
         <v>41610</v>
       </c>
       <c r="E45" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B46" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C46" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" s="7">
+        <v>41616</v>
+      </c>
+      <c r="E46" s="2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B47" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C47" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" s="7">
+        <v>41617</v>
+      </c>
+      <c r="E47" s="2">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B48" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" s="7">
+        <v>41618</v>
+      </c>
+      <c r="E48" s="2">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.25">
+      <c r="B49" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" s="7">
+        <v>41619</v>
+      </c>
+      <c r="E49" s="2">
         <v>1.5</v>
       </c>
     </row>

</xml_diff>